<commit_message>
Included new graphs and tables in paper and commented and adjusted the text in the paper
</commit_message>
<xml_diff>
--- a/src/results/descriptives/source_countries_shares_ftapp_and_dec.xlsx
+++ b/src/results/descriptives/source_countries_shares_ftapp_and_dec.xlsx
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:L15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>